<commit_message>
Update example game files.
</commit_message>
<xml_diff>
--- a/biosim_server_beta/example_game_ant.xlsx
+++ b/biosim_server_beta/example_game_ant.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20325"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shenshen Han\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{22E180C7-63DF-421C-B610-64D58AF7478A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="0" windowWidth="25600" windowHeight="15700" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1280" yWindow="0" windowWidth="25600" windowHeight="15700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="biosim-setup" sheetId="1" r:id="rId1"/>
@@ -18,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'biosim-setup'!$A$4:$W$12</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -246,13 +240,13 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>bee</t>
+    <t>ant</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -406,45 +400,45 @@
     </xf>
   </cellXfs>
   <cellStyles count="39">
-    <cellStyle name="超連結" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="超連結" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="超連結" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="超連結" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="超連結" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="超連結" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="超連結" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="超連結" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="超連結" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="超連結" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="超連結" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="超連結" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="超連結" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="超連結" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="超連結" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="超連結" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="超連結" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="超連結" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="超連結" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="一般" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="已瀏覽過的超連結" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="已瀏覽過的超連結" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="已瀏覽過的超連結" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="已瀏覽過的超連結" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="已瀏覽過的超連結" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="已瀏覽過的超連結" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="已瀏覽過的超連結" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="已瀏覽過的超連結" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="已瀏覽過的超連結" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="已瀏覽過的超連結" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="已瀏覽過的超連結" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="已瀏覽過的超連結" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="已瀏覽過的超連結" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="已瀏覽過的超連結" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="已瀏覽過的超連結" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="已瀏覽過的超連結" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="已瀏覽過的超連結" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="已瀏覽過的超連結" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="已瀏覽過的超連結" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="普通" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="37" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="86">
     <dxf>
@@ -1647,14 +1641,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" customWidth="1"/>
@@ -1675,7 +1669,7 @@
     <col min="23" max="23" width="18.1640625" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="56" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:23" ht="56" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1717,7 +1711,7 @@
       <c r="Q1" s="3"/>
       <c r="R1" s="3"/>
     </row>
-    <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" ht="15" customHeight="1">
       <c r="A2" s="7" t="s">
         <v>55</v>
       </c>
@@ -1759,7 +1753,7 @@
       <c r="Q2" s="3"/>
       <c r="R2" s="3"/>
     </row>
-    <row r="3" spans="1:23" ht="61" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" ht="61" customHeight="1">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1779,7 +1773,7 @@
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
     </row>
-    <row r="4" spans="1:23" s="1" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:23" s="1" customFormat="1" ht="55" customHeight="1">
       <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
@@ -1850,7 +1844,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" ht="15" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>24</v>
       </c>
@@ -1901,7 +1895,7 @@
       </c>
       <c r="W5" s="9"/>
     </row>
-    <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" ht="15" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>32</v>
       </c>
@@ -1949,7 +1943,7 @@
       <c r="V6" s="12"/>
       <c r="W6" s="9"/>
     </row>
-    <row r="7" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" ht="15" customHeight="1">
       <c r="A7" s="5"/>
       <c r="B7" s="6"/>
       <c r="C7" s="5"/>
@@ -1985,7 +1979,7 @@
       <c r="V7" s="12"/>
       <c r="W7" s="9"/>
     </row>
-    <row r="8" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" ht="15" customHeight="1">
       <c r="A8" s="5" t="s">
         <v>53</v>
       </c>
@@ -2035,7 +2029,7 @@
       <c r="V8" s="12"/>
       <c r="W8" s="9"/>
     </row>
-    <row r="9" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" ht="15" customHeight="1">
       <c r="A9" s="5" t="s">
         <v>39</v>
       </c>
@@ -2085,7 +2079,7 @@
       <c r="V9" s="12"/>
       <c r="W9" s="9"/>
     </row>
-    <row r="10" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" ht="15" customHeight="1">
       <c r="A10" s="5" t="s">
         <v>40</v>
       </c>
@@ -2135,7 +2129,7 @@
       <c r="V10" s="12"/>
       <c r="W10" s="9"/>
     </row>
-    <row r="11" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" ht="15" customHeight="1">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -2176,7 +2170,7 @@
       <c r="V11" s="12"/>
       <c r="W11" s="9"/>
     </row>
-    <row r="12" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" ht="15" customHeight="1">
       <c r="A12" s="5" t="s">
         <v>54</v>
       </c>
@@ -2224,7 +2218,7 @@
       <c r="V12" s="12"/>
       <c r="W12" s="9"/>
     </row>
-    <row r="13" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" ht="15" customHeight="1">
       <c r="A13" s="5" t="s">
         <v>54</v>
       </c>
@@ -2276,7 +2270,7 @@
       </c>
       <c r="W13" s="9"/>
     </row>
-    <row r="14" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" ht="15" customHeight="1">
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="C14" s="5"/>
@@ -2301,7 +2295,7 @@
       <c r="V14" s="12"/>
       <c r="W14" s="9"/>
     </row>
-    <row r="15" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" ht="15" customHeight="1">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -2329,7 +2323,7 @@
       <c r="V15" s="12"/>
       <c r="W15" s="9"/>
     </row>
-    <row r="16" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" ht="15" customHeight="1">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -2357,7 +2351,7 @@
       <c r="V16" s="12"/>
       <c r="W16" s="9"/>
     </row>
-    <row r="17" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" ht="15" customHeight="1">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -2385,7 +2379,7 @@
       <c r="V17" s="12"/>
       <c r="W17" s="9"/>
     </row>
-    <row r="18" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" ht="15" customHeight="1">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -2413,7 +2407,7 @@
       <c r="V18" s="12"/>
       <c r="W18" s="9"/>
     </row>
-    <row r="19" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" ht="15" customHeight="1">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -2441,7 +2435,7 @@
       <c r="V19" s="12"/>
       <c r="W19" s="9"/>
     </row>
-    <row r="20" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" ht="15" customHeight="1">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -2469,7 +2463,7 @@
       <c r="V20" s="12"/>
       <c r="W20" s="9"/>
     </row>
-    <row r="21" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" ht="15" customHeight="1">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -2497,7 +2491,7 @@
       <c r="V21" s="12"/>
       <c r="W21" s="9"/>
     </row>
-    <row r="22" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" ht="15" customHeight="1">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -2525,7 +2519,7 @@
       <c r="V22" s="12"/>
       <c r="W22" s="9"/>
     </row>
-    <row r="23" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" ht="15" customHeight="1">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -2553,7 +2547,7 @@
       <c r="V23" s="12"/>
       <c r="W23" s="9"/>
     </row>
-    <row r="24" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" ht="15" customHeight="1">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -2581,7 +2575,7 @@
       <c r="V24" s="12"/>
       <c r="W24" s="9"/>
     </row>
-    <row r="25" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" ht="15" customHeight="1">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -2609,7 +2603,7 @@
       <c r="V25" s="12"/>
       <c r="W25" s="9"/>
     </row>
-    <row r="26" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" ht="15" customHeight="1">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -2637,7 +2631,7 @@
       <c r="V26" s="12"/>
       <c r="W26" s="9"/>
     </row>
-    <row r="27" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" ht="15" customHeight="1">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -2665,7 +2659,7 @@
       <c r="V27" s="12"/>
       <c r="W27" s="9"/>
     </row>
-    <row r="28" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" ht="15" customHeight="1">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -2693,7 +2687,7 @@
       <c r="V28" s="12"/>
       <c r="W28" s="9"/>
     </row>
-    <row r="29" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" ht="15" customHeight="1">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -2721,7 +2715,7 @@
       <c r="V29" s="12"/>
       <c r="W29" s="9"/>
     </row>
-    <row r="30" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" ht="15" customHeight="1">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -2749,7 +2743,7 @@
       <c r="V30" s="12"/>
       <c r="W30" s="9"/>
     </row>
-    <row r="31" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" ht="15" customHeight="1">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -2777,7 +2771,7 @@
       <c r="V31" s="12"/>
       <c r="W31" s="9"/>
     </row>
-    <row r="32" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" ht="15" customHeight="1">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -2805,7 +2799,7 @@
       <c r="V32" s="12"/>
       <c r="W32" s="9"/>
     </row>
-    <row r="33" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" ht="15" customHeight="1">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -2833,7 +2827,7 @@
       <c r="V33" s="12"/>
       <c r="W33" s="9"/>
     </row>
-    <row r="34" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" ht="15" customHeight="1">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -2861,7 +2855,7 @@
       <c r="V34" s="12"/>
       <c r="W34" s="9"/>
     </row>
-    <row r="35" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" ht="15" customHeight="1">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -2889,7 +2883,7 @@
       <c r="V35" s="12"/>
       <c r="W35" s="9"/>
     </row>
-    <row r="36" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" ht="15" customHeight="1">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -2917,7 +2911,7 @@
       <c r="V36" s="12"/>
       <c r="W36" s="9"/>
     </row>
-    <row r="37" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" ht="15" customHeight="1">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -2945,7 +2939,7 @@
       <c r="V37" s="12"/>
       <c r="W37" s="9"/>
     </row>
-    <row r="38" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" ht="15" customHeight="1">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -2973,7 +2967,7 @@
       <c r="V38" s="12"/>
       <c r="W38" s="9"/>
     </row>
-    <row r="39" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" ht="15" customHeight="1">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -3001,7 +2995,7 @@
       <c r="V39" s="12"/>
       <c r="W39" s="9"/>
     </row>
-    <row r="40" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" ht="15" customHeight="1">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -3351,117 +3345,117 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="29">
-    <dataValidation type="whole" showErrorMessage="1" errorTitle="Space dimension not valid" error="Please enter a value between 10 and 100" sqref="D2" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="whole" showErrorMessage="1" errorTitle="Space dimension not valid" error="Please enter a value between 10 and 100" sqref="D2">
       <formula1>10</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C40" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C40">
       <formula1>1</formula1>
       <formula2>200</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B40" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B40">
       <formula1>"bee,hive,flower,fountain,ant"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J40" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J40">
       <formula1>"low,medium,high"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:E5" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:E5">
       <formula1>1</formula1>
       <formula2>B2-1</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:E6" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:E6">
       <formula1>1</formula1>
       <formula2>B2-1</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:E7" xr:uid="{00000000-0002-0000-0000-000006000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:E7">
       <formula1>1</formula1>
       <formula2>B2-1</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8:E8" xr:uid="{00000000-0002-0000-0000-000007000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8:E8">
       <formula1>1</formula1>
       <formula2>B2-1</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:E9" xr:uid="{00000000-0002-0000-0000-000008000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:E9">
       <formula1>1</formula1>
       <formula2>B2-1</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10:E10" xr:uid="{00000000-0002-0000-0000-000009000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10:E10">
       <formula1>1</formula1>
       <formula2>B2-1</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K5:K40 M5:M40" xr:uid="{00000000-0002-0000-0000-00000A000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K5:K40 M5:M40">
       <formula1>"none,slow,medium,fast"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P5:P40" xr:uid="{00000000-0002-0000-0000-00000B000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P5:P40">
       <formula1>"near,medium,far"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D11:E11" xr:uid="{00000000-0002-0000-0000-00000C000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D11:E11">
       <formula1>1</formula1>
       <formula2>B2-1</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D12:E12" xr:uid="{00000000-0002-0000-0000-00000D000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D12:E12">
       <formula1>1</formula1>
       <formula2>B2-1</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D13:E13" xr:uid="{00000000-0002-0000-0000-00000E000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D13:E13">
       <formula1>1</formula1>
       <formula2>B2-1</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D14:E14" xr:uid="{00000000-0002-0000-0000-00000F000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D14:E14">
       <formula1>1</formula1>
       <formula2>B2-1</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D15:E15" xr:uid="{00000000-0002-0000-0000-000010000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D15:E15">
       <formula1>1</formula1>
       <formula2>B2-1</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D16:E16" xr:uid="{00000000-0002-0000-0000-000011000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D16:E16">
       <formula1>1</formula1>
       <formula2>B2-1</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D17:E17" xr:uid="{00000000-0002-0000-0000-000012000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D17:E17">
       <formula1>1</formula1>
       <formula2>B2-1</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D18:E18" xr:uid="{00000000-0002-0000-0000-000013000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D18:E18">
       <formula1>1</formula1>
       <formula2>B2-1</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D19:E19 D21:E21 D23:E23 D25:E25 D27:E27 D29:E29 D31:E31 D33:E33 D35:E35 D37:E37 D39:E39" xr:uid="{00000000-0002-0000-0000-000014000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D19:E19 D21:E21 D23:E23 D25:E25 D27:E27 D29:E29 D31:E31 D33:E33 D35:E35 D37:E37 D39:E39">
       <formula1>1</formula1>
       <formula2>B2-1</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D20:E20 D22:E22 D24:E24 D26:E26 D28:E28 D30:E30 D32:E32 D34:E34 D36:E36 D38:E38 D40:E40" xr:uid="{00000000-0002-0000-0000-000015000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D20:E20 D22:E22 D24:E24 D26:E26 D28:E28 D30:E30 D32:E32 D34:E34 D36:E36 D38:E38 D40:E40">
       <formula1>1</formula1>
       <formula2>B2-1</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q5:Q40" xr:uid="{00000000-0002-0000-0000-000016000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q5:Q40">
       <formula1>"none,low,medium,high"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S5:S40" xr:uid="{00000000-0002-0000-0000-000017000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S5:S40">
       <formula1>"no,yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L5:L40 N5:N40" xr:uid="{00000000-0002-0000-0000-000018000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L5:L40 N5:N40">
       <formula1>"false,true"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O5:O40" xr:uid="{00000000-0002-0000-0000-000019000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O5:O40">
       <formula1>"flower,flower-2,flower-3,flower-4,flower-5,flower-6,flower-7,flower-8,flower-9,flower-10"</formula1>
     </dataValidation>
-    <dataValidation type="whole" showErrorMessage="1" errorTitle="Space dimension not valid" error="Please enter a value between 5 and 100" sqref="B2:C2" xr:uid="{00000000-0002-0000-0000-00001A000000}">
+    <dataValidation type="whole" showErrorMessage="1" errorTitle="Space dimension not valid" error="Please enter a value between 5 and 100" sqref="B2:C2">
       <formula1>4</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T1:U3 U5:U1048576 T41:T1048576" xr:uid="{00000000-0002-0000-0000-00001B000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T1:U3 U5:U1048576 T41:T1048576">
       <formula1>0</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T5:T40" xr:uid="{00000000-0002-0000-0000-00001C000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T5:T40">
       <formula1>2</formula1>
       <formula2>10</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Update ant game file.
</commit_message>
<xml_diff>
--- a/biosim_server_beta/example_game_ant.xlsx
+++ b/biosim_server_beta/example_game_ant.xlsx
@@ -1645,7 +1645,7 @@
   <dimension ref="A1:W40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -1716,10 +1716,10 @@
         <v>55</v>
       </c>
       <c r="B2" s="7">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C2" s="7">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D2" s="7">
         <v>70</v>
@@ -1731,10 +1731,10 @@
         <v>6</v>
       </c>
       <c r="G2" s="7">
-        <v>4.5</v>
+        <v>6.6</v>
       </c>
       <c r="H2" s="7">
-        <v>3.6</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I2" s="7">
         <v>30</v>

</xml_diff>